<commit_message>
added to docs, atempt at unity
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 1/SixGuys_Deliverable_1_ProductBackLog_1.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 1/SixGuys_Deliverable_1_ProductBackLog_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83E9929-F3ED-40D3-B6A3-0C3D5245FDD1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5FBEB-762F-4E46-8497-592C6DD4820A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
   </bookViews>
@@ -383,12 +383,11 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -421,19 +420,25 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F76"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -497,19 +502,11 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -525,18 +522,21 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F76"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -569,18 +569,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8479C2CE-F365-4119-A226-F6FAFAD8A4CF}" name="Table4" displayName="Table4" ref="A1:F25" totalsRowShown="0" headerRowDxfId="2" dataDxfId="5" headerRowCellStyle="Input">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8479C2CE-F365-4119-A226-F6FAFAD8A4CF}" name="Table4" displayName="Table4" ref="A1:F25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowCellStyle="Input">
   <autoFilter ref="A1:F25" xr:uid="{B185C55B-4D64-49B0-805A-90960E16F066}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
     <sortCondition ref="C2:C25" customList="H,M,L"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1FDADD91-D621-4F44-B591-C349E89B10F7}" name="Sprint Number" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{1FDADD91-D621-4F44-B591-C349E89B10F7}" name="Sprint Number" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{F07D2BD0-D352-48DB-BF4F-9202E12625B1}" name="ID" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{4187F81A-8072-4929-8F3E-AE2C49BCCB7A}" name="Story Priority" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{745801D7-6926-4CC7-AB96-9E52607BBB36}" name="Story Status" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{745801D7-6926-4CC7-AB96-9E52607BBB36}" name="Story Status" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{E9675B24-95C0-49EA-90BD-B361E90F2CBE}" name="Story Points" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{EE40AAE1-C44B-4B6D-A86A-8FAC1C8465A6}" name="User Story" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{EE40AAE1-C44B-4B6D-A86A-8FAC1C8465A6}" name="User Story" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1301,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
       <c r="B2" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updated documents for Deliverable 1
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 1/SixGuys_Deliverable_1_ProductBackLog_1.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 1/SixGuys_Deliverable_1_ProductBackLog_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5FBEB-762F-4E46-8497-592C6DD4820A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8DA613-605C-4AC7-8213-3DD5274A5A16}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -197,6 +197,27 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>As a player I want an enemy to go against me so that I feel more challenged.</t>
+  </si>
+  <si>
+    <t>GamePlay_8</t>
+  </si>
+  <si>
+    <t>Menu_Option_2</t>
+  </si>
+  <si>
+    <t>Menu_Option_3</t>
+  </si>
+  <si>
+    <t>Menu_Option_4</t>
+  </si>
+  <si>
+    <t>GamePlay_9</t>
+  </si>
+  <si>
+    <t>As a player I want to be able to shoot food so that I can defeat my enemies.</t>
   </si>
 </sst>
 </file>
@@ -284,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -335,12 +356,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -370,6 +426,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -569,10 +645,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8479C2CE-F365-4119-A226-F6FAFAD8A4CF}" name="Table4" displayName="Table4" ref="A1:F25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowCellStyle="Input">
-  <autoFilter ref="A1:F25" xr:uid="{B185C55B-4D64-49B0-805A-90960E16F066}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
-    <sortCondition ref="C2:C25" customList="H,M,L"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8479C2CE-F365-4119-A226-F6FAFAD8A4CF}" name="Table4" displayName="Table4" ref="A1:F27" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowCellStyle="Input">
+  <autoFilter ref="A1:F27" xr:uid="{B185C55B-4D64-49B0-805A-90960E16F066}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F26">
+    <sortCondition ref="C2:C26" customList="H,M,L"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1FDADD91-D621-4F44-B591-C349E89B10F7}" name="Sprint Number" dataDxfId="5"/>
@@ -1263,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5E4C9C-67CA-4794-82AA-DDD7FE2958B2}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1301,11 +1377,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
+      <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>53</v>
@@ -1317,14 +1391,14 @@
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>53</v>
@@ -1336,14 +1410,16 @@
         <v>13</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>53</v>
@@ -1352,17 +1428,17 @@
         <v>23</v>
       </c>
       <c r="E4" s="6">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>53</v>
@@ -1374,14 +1450,14 @@
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>53</v>
@@ -1390,10 +1466,10 @@
         <v>23</v>
       </c>
       <c r="E6" s="6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -1418,27 +1494,27 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>54</v>
+      <c r="B8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>54</v>
@@ -1447,17 +1523,17 @@
         <v>27</v>
       </c>
       <c r="E9" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>54</v>
@@ -1469,14 +1545,14 @@
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>54</v>
@@ -1488,14 +1564,14 @@
         <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>54</v>
@@ -1504,17 +1580,17 @@
         <v>27</v>
       </c>
       <c r="E12" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>54</v>
@@ -1523,17 +1599,17 @@
         <v>27</v>
       </c>
       <c r="E13" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>54</v>
@@ -1542,36 +1618,36 @@
         <v>27</v>
       </c>
       <c r="E14" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E15" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>29</v>
@@ -1580,17 +1656,17 @@
         <v>27</v>
       </c>
       <c r="E16" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>29</v>
@@ -1602,33 +1678,33 @@
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E18" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>29</v>
@@ -1637,17 +1713,17 @@
         <v>27</v>
       </c>
       <c r="E19" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>29</v>
@@ -1659,14 +1735,14 @@
         <v>2</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>29</v>
@@ -1675,17 +1751,17 @@
         <v>27</v>
       </c>
       <c r="E21" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>29</v>
@@ -1697,14 +1773,14 @@
         <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>29</v>
@@ -1713,17 +1789,17 @@
         <v>27</v>
       </c>
       <c r="E23" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>29</v>
@@ -1732,17 +1808,17 @@
         <v>27</v>
       </c>
       <c r="E24" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>29</v>
@@ -1754,17 +1830,52 @@
         <v>5</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="16">
+        <v>3</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="16">
+        <v>5</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed temp files, added to Sprint review doc
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 1/SixGuys_Deliverable_1_ProductBackLog_1.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 1/SixGuys_Deliverable_1_ProductBackLog_1.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D318D28E-3099-4BA3-9D90-9B9FAA63CA10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4896FC6D-6A5E-4786-9436-2A50739009A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10950" yWindow="390" windowWidth="17565" windowHeight="15180" activeTab="1" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Product backlog" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -681,23 +680,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DD0E1E96-69B8-420B-81DC-86D19F1C9F95}" name="Table2" displayName="Table2" ref="A1:F71" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F71">
-    <sortCondition ref="C2:C71" customList="H,M,L"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DCF50467-4650-4588-B607-3C391D683DA4}" name="Sprint Number"/>
-    <tableColumn id="2" xr3:uid="{886F9DD1-87FE-43CA-9389-324FCC208E3C}" name="ID"/>
-    <tableColumn id="3" xr3:uid="{F6415CEF-CBE7-4CD1-AE4F-583A2CCFC13C}" name="Story Priority"/>
-    <tableColumn id="4" xr3:uid="{9C520E79-18DF-4719-9F95-03A39A5A94DD}" name="Story Status"/>
-    <tableColumn id="5" xr3:uid="{9F3D408F-083E-4D40-AC32-B8E441BA352D}" name="Story Points"/>
-    <tableColumn id="6" xr3:uid="{3A5E4D20-71D9-4008-80EE-DD8B06AD3270}" name="User Story"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8479C2CE-F365-4119-A226-F6FAFAD8A4CF}" name="Table4" displayName="Table4" ref="A1:F34" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowCellStyle="Input">
   <autoFilter ref="A1:F34" xr:uid="{B185C55B-4D64-49B0-805A-90960E16F066}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F34">
@@ -1011,391 +993,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADBEB81-A78D-4C58-9D8E-F9E5223237E3}">
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="174.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5E4C9C-67CA-4794-82AA-DDD7FE2958B2}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1430,7 +1032,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
       <c r="B2" s="5" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1053,9 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
       <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
@@ -1489,7 +1095,9 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
       <c r="B5" s="17" t="s">
         <v>74</v>
       </c>
@@ -1508,7 +1116,9 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
       <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
@@ -1546,7 +1156,9 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
       <c r="B8" s="5" t="s">
         <v>44</v>
       </c>

</xml_diff>